<commit_message>
fix error in oracle
</commit_message>
<xml_diff>
--- a/test_cases/modified_oracle/gentests_t2_oracle.xlsx
+++ b/test_cases/modified_oracle/gentests_t2_oracle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinizr\phd\courses\gssi_testing\exam\essay\ct4bsn-replication_package\test_cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinizr\phd\courses\gssi_testing\exam\essay\ct4bsn-replication_package\test_cases\modified_oracle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0BD0CBF1-D824-46BB-A05F-F265FBD68724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A90146-749A-4438-BE70-59D44F04F675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BSN-Test Set" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -471,11 +471,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -638,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <f>IF(IF(B8&gt;3,1,0)+IF(D8&gt;3,1,0)+IF(F8&gt;3,1,0)+IF(H8&gt;3,1,0)+IF(J8&gt;3,1,0)+IF(L8&gt;3,1,0)&gt;0,"ERROR",0)</f>
+        <f>IF(IF(B8*C8&gt;3,1,0)+IF(D8*E8&gt;3,1,0)+IF(F8*G8&gt;3,1,0)+IF(H8*I8&gt;3,1,0)+IF(J8*K8&gt;3,1,0)+IF(L8*M8&gt;3,1,0)&gt;0,"ERROR",0)</f>
         <v>0</v>
       </c>
       <c r="T8">
@@ -711,7 +711,7 @@
         <v>100</v>
       </c>
       <c r="S9">
-        <f t="shared" ref="S9:S72" si="1">IF(IF(B9&gt;3,1,0)+IF(D9&gt;3,1,0)+IF(F9&gt;3,1,0)+IF(H9&gt;3,1,0)+IF(J9&gt;3,1,0)+IF(L9&gt;3,1,0)&gt;0,"ERROR",0)</f>
+        <f t="shared" ref="S9:S72" si="1">IF(IF(B9*C9&gt;3,1,0)+IF(D9*E9&gt;3,1,0)+IF(F9*G9&gt;3,1,0)+IF(H9*I9&gt;3,1,0)+IF(J9*K9&gt;3,1,0)+IF(L9*M9&gt;3,1,0)&gt;0,"ERROR",0)</f>
         <v>0</v>
       </c>
       <c r="T9">
@@ -2535,21 +2535,21 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S34" t="str">
+      <c r="S34">
         <f t="shared" si="1"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T34">
         <f t="shared" si="4"/>
         <v>1.04</v>
       </c>
-      <c r="U34" t="str">
+      <c r="U34">
         <f t="shared" si="2"/>
-        <v>Invalid</v>
+        <v>0</v>
       </c>
       <c r="V34" t="str">
         <f t="shared" si="3"/>
-        <v>Critical</v>
+        <v>No Risk</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
@@ -2754,21 +2754,21 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S37" t="str">
+      <c r="S37">
         <f t="shared" si="1"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T37">
         <f t="shared" si="4"/>
         <v>1.1600000000000001</v>
       </c>
-      <c r="U37" t="str">
+      <c r="U37">
         <f t="shared" si="2"/>
-        <v>Invalid</v>
+        <v>0</v>
       </c>
       <c r="V37" t="str">
         <f t="shared" si="3"/>
-        <v>Critical</v>
+        <v>No Risk</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
@@ -2900,21 +2900,21 @@
         <f t="shared" si="5"/>
         <v>33.333333333333329</v>
       </c>
-      <c r="S39" t="str">
+      <c r="S39">
         <f t="shared" si="1"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T39">
         <f t="shared" si="4"/>
         <v>1.0900000000000001</v>
       </c>
-      <c r="U39" t="str">
+      <c r="U39">
         <f t="shared" si="2"/>
-        <v>Invalid</v>
+        <v>36.333333333333329</v>
       </c>
       <c r="V39" t="str">
         <f t="shared" si="3"/>
-        <v>Critical</v>
+        <v>Low Risk</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
@@ -3046,17 +3046,17 @@
         <f t="shared" si="5"/>
         <v>100</v>
       </c>
-      <c r="S41" t="str">
+      <c r="S41">
         <f t="shared" si="1"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T41">
         <f t="shared" si="4"/>
         <v>1.0899999999999999</v>
       </c>
-      <c r="U41" t="str">
+      <c r="U41">
         <f t="shared" si="2"/>
-        <v>Invalid</v>
+        <v>108.99999999999999</v>
       </c>
       <c r="V41" t="str">
         <f t="shared" si="3"/>
@@ -3265,17 +3265,17 @@
         <f t="shared" si="5"/>
         <v>100</v>
       </c>
-      <c r="S44" t="str">
+      <c r="S44">
         <f t="shared" si="1"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T44">
         <f t="shared" si="4"/>
         <v>1.21</v>
       </c>
-      <c r="U44" t="str">
+      <c r="U44">
         <f t="shared" si="2"/>
-        <v>Invalid</v>
+        <v>121</v>
       </c>
       <c r="V44" t="str">
         <f t="shared" si="3"/>
@@ -3338,21 +3338,21 @@
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
-      <c r="S45" t="str">
+      <c r="S45">
         <f t="shared" si="1"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T45">
         <f t="shared" si="4"/>
         <v>0.99</v>
       </c>
-      <c r="U45" t="str">
+      <c r="U45">
         <f t="shared" si="2"/>
-        <v>Invalid</v>
+        <v>49.5</v>
       </c>
       <c r="V45" t="str">
         <f t="shared" si="3"/>
-        <v>Critical</v>
+        <v>Moderate</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
@@ -3484,17 +3484,17 @@
         <f t="shared" si="5"/>
         <v>100</v>
       </c>
-      <c r="S47" t="str">
+      <c r="S47">
         <f t="shared" si="1"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T47">
         <f t="shared" si="4"/>
         <v>1.17</v>
       </c>
-      <c r="U47" t="str">
+      <c r="U47">
         <f t="shared" si="2"/>
-        <v>Invalid</v>
+        <v>117</v>
       </c>
       <c r="V47" t="str">
         <f t="shared" si="3"/>
@@ -3557,21 +3557,21 @@
         <f t="shared" si="5"/>
         <v>33.333333333333329</v>
       </c>
-      <c r="S48" t="str">
+      <c r="S48">
         <f t="shared" si="1"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T48">
         <f t="shared" si="4"/>
         <v>1.1100000000000001</v>
       </c>
-      <c r="U48" t="str">
+      <c r="U48">
         <f t="shared" si="2"/>
-        <v>Invalid</v>
+        <v>37</v>
       </c>
       <c r="V48" t="str">
         <f t="shared" si="3"/>
-        <v>Critical</v>
+        <v>Low Risk</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
@@ -3703,17 +3703,17 @@
         <f t="shared" si="5"/>
         <v>100</v>
       </c>
-      <c r="S50" t="str">
+      <c r="S50">
         <f t="shared" si="1"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T50">
         <f t="shared" si="4"/>
         <v>1.2849999999999999</v>
       </c>
-      <c r="U50" t="str">
+      <c r="U50">
         <f t="shared" si="2"/>
-        <v>Invalid</v>
+        <v>128.5</v>
       </c>
       <c r="V50" t="str">
         <f t="shared" si="3"/>
@@ -4798,21 +4798,21 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S65" t="str">
+      <c r="S65">
         <f t="shared" si="1"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T65">
         <f t="shared" si="4"/>
         <v>1.0899999999999999</v>
       </c>
-      <c r="U65" t="str">
+      <c r="U65">
         <f t="shared" si="2"/>
-        <v>Invalid</v>
+        <v>0</v>
       </c>
       <c r="V65" t="str">
         <f t="shared" si="3"/>
-        <v>Critical</v>
+        <v>No Risk</v>
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
@@ -5017,21 +5017,21 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S68" t="str">
+      <c r="S68">
         <f t="shared" si="1"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T68">
         <f t="shared" si="4"/>
         <v>1.21</v>
       </c>
-      <c r="U68" t="str">
+      <c r="U68">
         <f t="shared" si="2"/>
-        <v>Invalid</v>
+        <v>0</v>
       </c>
       <c r="V68" t="str">
         <f t="shared" si="3"/>
-        <v>Critical</v>
+        <v>No Risk</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.25">
@@ -5163,21 +5163,21 @@
         <f t="shared" si="5"/>
         <v>55.555555555555557</v>
       </c>
-      <c r="S70" t="str">
+      <c r="S70">
         <f t="shared" si="1"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T70">
         <f t="shared" si="4"/>
         <v>1.0900000000000001</v>
       </c>
-      <c r="U70" t="str">
+      <c r="U70">
         <f t="shared" si="2"/>
-        <v>Invalid</v>
+        <v>60.555555555555564</v>
       </c>
       <c r="V70" t="str">
         <f t="shared" si="3"/>
-        <v>Critical</v>
+        <v>Risky</v>
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
@@ -5309,21 +5309,21 @@
         <f t="shared" si="5"/>
         <v>33.333333333333329</v>
       </c>
-      <c r="S72" t="str">
+      <c r="S72">
         <f t="shared" si="1"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T72">
         <f t="shared" si="4"/>
         <v>1.1099999999999999</v>
       </c>
-      <c r="U72" t="str">
+      <c r="U72">
         <f t="shared" si="2"/>
-        <v>Invalid</v>
+        <v>36.999999999999993</v>
       </c>
       <c r="V72" t="str">
         <f t="shared" si="3"/>
-        <v>Critical</v>
+        <v>Low Risk</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
@@ -5383,7 +5383,7 @@
         <v>66.666666666666657</v>
       </c>
       <c r="S73" t="str">
-        <f t="shared" ref="S73:S105" si="6">IF(IF(B73&gt;3,1,0)+IF(D73&gt;3,1,0)+IF(F73&gt;3,1,0)+IF(H73&gt;3,1,0)+IF(J73&gt;3,1,0)+IF(L73&gt;3,1,0)&gt;0,"ERROR",0)</f>
+        <f t="shared" ref="S73:S105" si="6">IF(IF(B73*C73&gt;3,1,0)+IF(D73*E73&gt;3,1,0)+IF(F73*G73&gt;3,1,0)+IF(H73*I73&gt;3,1,0)+IF(J73*K73&gt;3,1,0)+IF(L73*M73&gt;3,1,0)&gt;0,"ERROR",0)</f>
         <v>ERROR</v>
       </c>
       <c r="T73">
@@ -6477,21 +6477,21 @@
         <f t="shared" si="10"/>
         <v>33.333333333333329</v>
       </c>
-      <c r="S88" t="str">
+      <c r="S88">
         <f t="shared" si="6"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T88">
         <f t="shared" si="9"/>
         <v>1.01</v>
       </c>
-      <c r="U88" t="str">
+      <c r="U88">
         <f t="shared" si="7"/>
-        <v>Invalid</v>
+        <v>33.666666666666664</v>
       </c>
       <c r="V88" t="str">
         <f t="shared" si="8"/>
-        <v>Critical</v>
+        <v>Low Risk</v>
       </c>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.25">
@@ -6550,21 +6550,21 @@
         <f t="shared" si="10"/>
         <v>46.666666666666664</v>
       </c>
-      <c r="S89" t="str">
+      <c r="S89">
         <f t="shared" si="6"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T89">
         <f t="shared" si="9"/>
         <v>1.03</v>
       </c>
-      <c r="U89" t="str">
+      <c r="U89">
         <f t="shared" si="7"/>
-        <v>Invalid</v>
+        <v>48.066666666666663</v>
       </c>
       <c r="V89" t="str">
         <f t="shared" si="8"/>
-        <v>Critical</v>
+        <v>Moderate</v>
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.25">
@@ -6696,21 +6696,21 @@
         <f t="shared" si="10"/>
         <v>41.666666666666671</v>
       </c>
-      <c r="S91" t="str">
+      <c r="S91">
         <f t="shared" si="6"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T91">
         <f t="shared" si="9"/>
         <v>1.2</v>
       </c>
-      <c r="U91" t="str">
+      <c r="U91">
         <f t="shared" si="7"/>
-        <v>Invalid</v>
+        <v>50.000000000000007</v>
       </c>
       <c r="V91" t="str">
         <f t="shared" si="8"/>
-        <v>Critical</v>
+        <v>Moderate</v>
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.25">
@@ -6769,21 +6769,21 @@
         <f t="shared" si="10"/>
         <v>44.444444444444443</v>
       </c>
-      <c r="S92" t="str">
+      <c r="S92">
         <f t="shared" si="6"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T92">
         <f t="shared" si="9"/>
         <v>1.19</v>
       </c>
-      <c r="U92" t="str">
+      <c r="U92">
         <f t="shared" si="7"/>
-        <v>Invalid</v>
+        <v>52.888888888888886</v>
       </c>
       <c r="V92" t="str">
         <f t="shared" si="8"/>
-        <v>Critical</v>
+        <v>Moderate</v>
       </c>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.25">
@@ -6988,21 +6988,21 @@
         <f t="shared" si="10"/>
         <v>58.333333333333336</v>
       </c>
-      <c r="S95" t="str">
+      <c r="S95">
         <f t="shared" si="6"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T95">
         <f t="shared" si="9"/>
         <v>1.04</v>
       </c>
-      <c r="U95" t="str">
+      <c r="U95">
         <f t="shared" si="7"/>
-        <v>Invalid</v>
+        <v>60.666666666666671</v>
       </c>
       <c r="V95" t="str">
         <f t="shared" si="8"/>
-        <v>Critical</v>
+        <v>Risky</v>
       </c>
     </row>
     <row r="96" spans="1:22" x14ac:dyDescent="0.25">
@@ -7061,21 +7061,21 @@
         <f t="shared" si="10"/>
         <v>40</v>
       </c>
-      <c r="S96" t="str">
+      <c r="S96">
         <f t="shared" si="6"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T96">
         <f t="shared" si="9"/>
         <v>1.1299999999999999</v>
       </c>
-      <c r="U96" t="str">
+      <c r="U96">
         <f t="shared" si="7"/>
-        <v>Invalid</v>
+        <v>45.199999999999996</v>
       </c>
       <c r="V96" t="str">
         <f t="shared" si="8"/>
-        <v>Critical</v>
+        <v>Moderate</v>
       </c>
     </row>
     <row r="97" spans="1:22" x14ac:dyDescent="0.25">
@@ -7353,21 +7353,21 @@
         <f t="shared" si="10"/>
         <v>33.333333333333329</v>
       </c>
-      <c r="S100" t="str">
+      <c r="S100">
         <f t="shared" si="6"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T100">
         <f t="shared" si="9"/>
         <v>1.07</v>
       </c>
-      <c r="U100" t="str">
+      <c r="U100">
         <f t="shared" si="7"/>
-        <v>Invalid</v>
+        <v>35.666666666666664</v>
       </c>
       <c r="V100" t="str">
         <f t="shared" si="8"/>
-        <v>Critical</v>
+        <v>Low Risk</v>
       </c>
     </row>
     <row r="101" spans="1:22" x14ac:dyDescent="0.25">
@@ -7499,21 +7499,21 @@
         <f t="shared" si="10"/>
         <v>33.333333333333329</v>
       </c>
-      <c r="S102" t="str">
+      <c r="S102">
         <f t="shared" si="6"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T102">
         <f t="shared" si="9"/>
         <v>1.1600000000000001</v>
       </c>
-      <c r="U102" t="str">
+      <c r="U102">
         <f t="shared" si="7"/>
-        <v>Invalid</v>
+        <v>38.666666666666664</v>
       </c>
       <c r="V102" t="str">
         <f t="shared" si="8"/>
-        <v>Critical</v>
+        <v>Low Risk</v>
       </c>
     </row>
     <row r="103" spans="1:22" x14ac:dyDescent="0.25">
@@ -7718,21 +7718,21 @@
         <f t="shared" si="10"/>
         <v>26.666666666666668</v>
       </c>
-      <c r="S105" t="str">
+      <c r="S105">
         <f t="shared" si="6"/>
-        <v>ERROR</v>
+        <v>0</v>
       </c>
       <c r="T105">
         <f t="shared" si="9"/>
         <v>1.2449999999999999</v>
       </c>
-      <c r="U105" t="str">
+      <c r="U105">
         <f t="shared" si="7"/>
-        <v>Invalid</v>
+        <v>33.199999999999996</v>
       </c>
       <c r="V105" t="str">
         <f t="shared" si="8"/>
-        <v>Critical</v>
+        <v>Low Risk</v>
       </c>
     </row>
   </sheetData>

</xml_diff>